<commit_message>
Add pydantic model gen; improve schema
Schema
- add slot: pid_schema_version
- fix: Make ResourceInfo single-valued
- style: Gave enums singular name
</commit_message>
<xml_diff>
--- a/project/excel/pid4cat_model.xlsx
+++ b/project/excel/pid4cat_model.xlsx
@@ -12,6 +12,7 @@
     <sheet name="ResourceInfo" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="LogRecord" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Agent" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Container" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -417,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,25 +444,35 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>record_version</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>pid_schema_version</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>dc_rights</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>curation_contact</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>resource_info</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>related_identifiers</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>dc_rights</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>curation_contact</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>change_log</t>
         </is>
@@ -509,14 +520,14 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>agent</t>
+          <t>has_agent</t>
         </is>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"IS_CITED_BY,CITES,IS_SUPPLEMENT_TO,IS_SUPPLEMENTED_BY,IS_CONTINUED_BY,CONTINUES,HAS_METADATA,IS_METADATA_FOR,HAS_VERSION,IS_VERSION_OF,IS_NEW_VERSION_OF,IS_PREVIOUS_VERSION_OF,IS_PART_OF,HAS_PART,IS_DESCRIBED_BY,DESCRIBES,IS_PUBLISHED_IN,IS_REFERENCED_BY,REFERENCES,IS_DOCUMENTED_BY,DOCUMENTS,IS_COMPILED_BY,COMPILES,IS_VARIANT_FORM_OF,IS_ORIGINAL_FORM_OF,IS_IDENTICAL_TO,IS_DERIVED_FROM,IS_SOURCE_OF,IS_REQUIRED_BY,REQUIRES,IS_OBSOLETED_BY,OBSOLETES"</formula1>
+      <formula1>"IS_CITED_BY,CITES,IS_SUPPLEMENT_TO,IS_SUPPLEMENTED_BY,IS_CONTINUED_BY,CONTINUES,HAS_METADATA,IS_METADATA_FOR,HAS_VERSION,IS_VERSION_OF,IS_NEW_VERSION_OF,IS_PREVIOUS_VERSION_OF,IS_PART_OF,HAS_PART,IS_DESCRIBED_BY,DESCRIBES,IS_PUBLISHED_IN,IS_REFERENCED_BY,REFERENCES,IS_DOCUMENTED_BY,DOCUMENTS,IS_COMPILED_BY,COMPILES,IS_VARIANT_FORM_OF,IS_ORIGINAL_FORM_OF,IS_IDENTICAL_TO,IS_DERIVED_FROM,IS_SOURCE_OF,IS_COLLECTED_BY,COLLECTS,IS_REQUIRED_BY,REQUIRES,IS_OBSOLETED_BY,OBSOLETES"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -577,7 +588,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"COLLECTION,CATALYST,MATERIAL,DEVICE,DATAOBJECT"</formula1>
+      <formula1>"COLLECTION,SAMPLE,MATERIAL,DEVICE,DATAOBJECT"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -606,7 +617,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>agent</t>
+          <t>has_agent</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -679,4 +690,30 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>contains_pids</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update template & dependencies
</commit_message>
<xml_diff>
--- a/project/excel/pid4cat_model.xlsx
+++ b/project/excel/pid4cat_model.xlsx
@@ -525,11 +525,6 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"IS_CITED_BY,CITES,IS_SUPPLEMENT_TO,IS_SUPPLEMENTED_BY,IS_CONTINUED_BY,CONTINUES,HAS_METADATA,IS_METADATA_FOR,HAS_VERSION,IS_VERSION_OF,IS_NEW_VERSION_OF,IS_PREVIOUS_VERSION_OF,IS_PART_OF,HAS_PART,IS_DESCRIBED_BY,DESCRIBES,IS_PUBLISHED_IN,IS_REFERENCED_BY,REFERENCES,IS_DOCUMENTED_BY,DOCUMENTS,IS_COMPILED_BY,COMPILES,IS_VARIANT_FORM_OF,IS_ORIGINAL_FORM_OF,IS_IDENTICAL_TO,IS_DERIVED_FROM,IS_SOURCE_OF,IS_COLLECTED_BY,COLLECTS,IS_REQUIRED_BY,REQUIRES,IS_OBSOLETED_BY,OBSOLETES"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Merge re-generated project files
</commit_message>
<xml_diff>
--- a/project/excel/pid4cat_model.xlsx
+++ b/project/excel/pid4cat_model.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,35 +444,30 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>record_version</t>
+          <t>pid_schema_version</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>pid_schema_version</t>
+          <t>license</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>dc_rights</t>
+          <t>curation_contact_email</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>curation_contact</t>
+          <t>resource_info</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>resource_info</t>
+          <t>related_identifiers</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
-        <is>
-          <t>related_identifiers</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
         <is>
           <t>change_log</t>
         </is>
@@ -583,7 +578,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"COLLECTION,SAMPLE,MATERIAL,DEVICE,DATAOBJECT"</formula1>
+      <formula1>"COLLECTION,SAMPLE,MATERIAL,DEVICE,DATA_OBJECT,DATA_SERVICE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -629,7 +624,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"STATUS,RESOURCE_INFO,RELATED_IDS,CONTACT,RIGHTS"</formula1>
+      <formula1>"STATUS,RESOURCE_INFO,RELATED_IDS,CONTACT,LICENSE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -658,12 +653,12 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>contact_information</t>
+          <t>email</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>person_orcid</t>
+          <t>orcid</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">

</xml_diff>

<commit_message>
Update examples & generated files after schema change
</commit_message>
<xml_diff>
--- a/project/excel/pid4cat_model.xlsx
+++ b/project/excel/pid4cat_model.xlsx
@@ -12,7 +12,8 @@
     <sheet name="ResourceInfo" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="LogRecord" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Agent" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Container" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="RepresentationVariant" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Container" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -530,7 +531,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,22 +557,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>rdf_url</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>schema_url</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>schema_type</t>
+          <t>representation_variants</t>
         </is>
       </c>
     </row>
@@ -688,6 +674,47 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>media_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>encoding_format</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>size</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Model: remove redundant info & add enum element
Removes has_agent from PID4CatRelation
Adds "LANDING_PAGE" to ChangeLogField enum
</commit_message>
<xml_diff>
--- a/project/excel/pid4cat_model.xlsx
+++ b/project/excel/pid4cat_model.xlsx
@@ -490,7 +490,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,11 +512,6 @@
       <c r="C1" t="inlineStr">
         <is>
           <t>datetime_log</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_agent</t>
         </is>
       </c>
     </row>
@@ -610,7 +605,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"STATUS,RESOURCE_INFO,RELATED_IDS,CONTACT,LICENSE"</formula1>
+      <formula1>"STATUS,LANDING_PAGE,RESOURCE_INFO,RELATED_IDS,CONTACT,LICENSE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Change model to closely match handle-API
</commit_message>
<xml_diff>
--- a/project/excel/pid4cat_model.xlsx
+++ b/project/excel/pid4cat_model.xlsx
@@ -7,13 +7,15 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="PID4CatRecord" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="PID4CatRelation" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="ResourceInfo" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="LogRecord" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Agent" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="RepresentationVariant" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Container" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="HandleAPIRecord" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="HandleRecord" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="HandleData" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="HandleRecordContainer" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="PID4CatRelation" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="ResourceInfo" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="LogRecord" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Agent" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="RepresentationVariant" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -419,72 +421,145 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>response_code</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>landing_page_url</t>
+          <t>handle</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>status</t>
+          <t>values</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>data</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>pid_schema_version</t>
+          <t>ttl</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>license</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>curation_contact_email</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>resource_info</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>related_identifiers</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>change_log</t>
+          <t>timestamp</t>
         </is>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"SUBMITTED,REGISTERED,OBSOLETED,DEPRECATED"</formula1>
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"URL,STATUS,SCHEMA_VER,LICENSE,EMAIL,RESOURCE_INFO,RELATED,LOG"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>contains_pids</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -520,7 +595,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -566,7 +641,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -612,7 +687,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -663,7 +738,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -702,30 +777,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>contains_pids</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update generated project artifacts
</commit_message>
<xml_diff>
--- a/project/excel/pid4cat_model.xlsx
+++ b/project/excel/pid4cat_model.xlsx
@@ -9,13 +9,36 @@
   <sheets>
     <sheet name="HandleAPIRecord" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="HandleRecord" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="HandleData" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="HandleRecordContainer" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Pid4CatRelation" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="ResourceInfo" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="LogRecord" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Agent" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="RepresentationVariant" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="URL" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="HdlDataUrl" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="STATUS" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="HdlDataStatus" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="SCHEMA_VER" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="HdlDataSchemaVer" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="LICENSE" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="HdlDataLicense" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="EMAIL" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="HdlDataContact" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="RESOURCE_INFO" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="HdlDataResourceInfo" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="RELATED" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="HdlDataRelated" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="LOG" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="HdlDataLog" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="HandleRecordContainer" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="Pid4CatRelation" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="ResourceInfo" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="LogRecord" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="Agent" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="RepresentationVariant" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="RelatedIdentifier" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="PurlIdentifier" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="DoiIdentifier" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="HandleIdentifier" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="ArkIdentifier" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="UrnIdentifier" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="GtinIdentifier" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="ExampleIdentifier" sheetId="32" state="visible" r:id="rId32"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -432,7 +455,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>response_code</t>
+          <t>responseCode</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -451,115 +474,408 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>data</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ttl</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>data</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ttl</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>data</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ttl</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>data</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ttl</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>contains_pids</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>index</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ttl</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>data</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>ttl</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>timestamp</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"URL,STATUS,SCHEMA_VER,LICENSE,EMAIL,RESOURCE_INFO,RELATED,LOG"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>format</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>contains_pids</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -595,7 +911,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -641,7 +957,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -680,14 +996,14 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"STATUS,LANDING_PAGE,RESOURCE_INFO,RELATED_IDS,CONTACT,LICENSE"</formula1>
+      <formula1>"STATUS,LANDING_PAGE,RESOURCE_INFO,RELATED_IDS,CONTACT,LICENSE,SCHEMA_VER"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -738,39 +1054,584 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>media_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>encoding_format</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>size</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>resolving_url</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>resolving_url</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>resolving_url</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>resolving_url</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>data</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ttl</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>resolving_url</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>data</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ttl</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"SUBMITTED,REGISTERED,OBSOLETED,DEPRECATED"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>data</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ttl</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>url</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>media_type</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>encoding_format</t>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>data</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ttl</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>size</t>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update generated project files
</commit_message>
<xml_diff>
--- a/project/excel/pid4cat_model.xlsx
+++ b/project/excel/pid4cat_model.xlsx
@@ -23,7 +23,7 @@
     <sheet name="HdlDataResourceInfo" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="RELATED" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="HdlDataRelated" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="LOG" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="CHANGES" sheetId="17" state="visible" r:id="rId17"/>
     <sheet name="HdlDataLog" sheetId="18" state="visible" r:id="rId18"/>
     <sheet name="HandleRecordContainer" sheetId="19" state="visible" r:id="rId19"/>
     <sheet name="Pid4CatRelation" sheetId="20" state="visible" r:id="rId20"/>
@@ -1025,7 +1025,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>email</t>
+          <t>email_address</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -1071,7 +1071,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>url</t>
+          <t>variant_url</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">

</xml_diff>

<commit_message>
Update auto-created model artifacts
</commit_message>
<xml_diff>
--- a/project/excel/pid4cat_model.xlsx
+++ b/project/excel/pid4cat_model.xlsx
@@ -39,6 +39,7 @@
     <sheet name="UrnIdentifier" sheetId="30" state="visible" r:id="rId30"/>
     <sheet name="GtinIdentifier" sheetId="31" state="visible" r:id="rId31"/>
     <sheet name="ExampleIdentifier" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="Pid4CatRecord" sheetId="33" state="visible" r:id="rId33"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1404,183 +1405,59 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>format</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>index</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>data</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>timestamp</t>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>landing_page_url</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>schema_version</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>ttl</t>
+          <t>metadata_license</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>format</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>index</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>data</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>timestamp</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>ttl</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>format</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>value</t>
+          <t>curation_contact</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>resource_info</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>related_identifiers</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>change_log</t>
         </is>
       </c>
     </row>
@@ -1594,6 +1471,196 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>data</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>ttl</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>data</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>ttl</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"SUBMITTED,REGISTERED,OBSOLETED,DEPRECATED"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>